<commit_message>
Kafka Script has been added
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/Transaction Details.xlsx
+++ b/src/test/resources/TestDataFiles/Transaction Details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="871">
   <si>
     <t>TRANSACTION ID</t>
   </si>
@@ -2390,6 +2390,249 @@
   </si>
   <si>
     <t>03:46:59:385</t>
+  </si>
+  <si>
+    <t>TR20240730011858230</t>
+  </si>
+  <si>
+    <t>01:18:58:231</t>
+  </si>
+  <si>
+    <t>TR20240730011858349</t>
+  </si>
+  <si>
+    <t>01:18:58:349</t>
+  </si>
+  <si>
+    <t>TR20240730011858459</t>
+  </si>
+  <si>
+    <t>01:18:58:460</t>
+  </si>
+  <si>
+    <t>TR20240731011858569</t>
+  </si>
+  <si>
+    <t>31-07-2024</t>
+  </si>
+  <si>
+    <t>01:18:58:569</t>
+  </si>
+  <si>
+    <t>TR20240731011858678</t>
+  </si>
+  <si>
+    <t>01:18:58:678</t>
+  </si>
+  <si>
+    <t>TR20240730012206941</t>
+  </si>
+  <si>
+    <t>01:22:06:941</t>
+  </si>
+  <si>
+    <t>TR20240730012207063</t>
+  </si>
+  <si>
+    <t>01:22:07:064</t>
+  </si>
+  <si>
+    <t>TR20240730012207172</t>
+  </si>
+  <si>
+    <t>01:22:07:173</t>
+  </si>
+  <si>
+    <t>TR20240731012207294</t>
+  </si>
+  <si>
+    <t>01:22:07:294</t>
+  </si>
+  <si>
+    <t>TR20240731012207403</t>
+  </si>
+  <si>
+    <t>01:22:07:404</t>
+  </si>
+  <si>
+    <t>TR20240730012655659</t>
+  </si>
+  <si>
+    <t>01:26:55:661</t>
+  </si>
+  <si>
+    <t>TR20240730012655780</t>
+  </si>
+  <si>
+    <t>01:26:55:782</t>
+  </si>
+  <si>
+    <t>TR20240730012655890</t>
+  </si>
+  <si>
+    <t>01:26:55:890</t>
+  </si>
+  <si>
+    <t>TR20240731012655994</t>
+  </si>
+  <si>
+    <t>01:26:55:994</t>
+  </si>
+  <si>
+    <t>TR20240731012656102</t>
+  </si>
+  <si>
+    <t>01:26:56:103</t>
+  </si>
+  <si>
+    <t>TR20240730013110530</t>
+  </si>
+  <si>
+    <t>01:31:10:531</t>
+  </si>
+  <si>
+    <t>TR20240730013110649</t>
+  </si>
+  <si>
+    <t>01:31:10:650</t>
+  </si>
+  <si>
+    <t>TR20240730013110761</t>
+  </si>
+  <si>
+    <t>01:31:10:762</t>
+  </si>
+  <si>
+    <t>TR20240731013110869</t>
+  </si>
+  <si>
+    <t>01:31:10:870</t>
+  </si>
+  <si>
+    <t>TR20240731013110977</t>
+  </si>
+  <si>
+    <t>01:31:10:977</t>
+  </si>
+  <si>
+    <t>TR20240730013307193</t>
+  </si>
+  <si>
+    <t>01:33:07:193</t>
+  </si>
+  <si>
+    <t>TR20240730013307312</t>
+  </si>
+  <si>
+    <t>01:33:07:312</t>
+  </si>
+  <si>
+    <t>TR20240730013307420</t>
+  </si>
+  <si>
+    <t>01:33:07:420</t>
+  </si>
+  <si>
+    <t>TR20240731013307529</t>
+  </si>
+  <si>
+    <t>01:33:07:530</t>
+  </si>
+  <si>
+    <t>TR20240731013307639</t>
+  </si>
+  <si>
+    <t>01:33:07:639</t>
+  </si>
+  <si>
+    <t>TR20240730014302717</t>
+  </si>
+  <si>
+    <t>01:43:02:718</t>
+  </si>
+  <si>
+    <t>TR20240730014302833</t>
+  </si>
+  <si>
+    <t>01:43:02:833</t>
+  </si>
+  <si>
+    <t>TR20240730014302939</t>
+  </si>
+  <si>
+    <t>01:43:02:939</t>
+  </si>
+  <si>
+    <t>TR20240731014303049</t>
+  </si>
+  <si>
+    <t>01:43:03:049</t>
+  </si>
+  <si>
+    <t>TR20240731014303154</t>
+  </si>
+  <si>
+    <t>01:43:03:154</t>
+  </si>
+  <si>
+    <t>TR20240730014724922</t>
+  </si>
+  <si>
+    <t>01:47:24:922</t>
+  </si>
+  <si>
+    <t>TR20240730014725038</t>
+  </si>
+  <si>
+    <t>01:47:25:038</t>
+  </si>
+  <si>
+    <t>TR20240730014725145</t>
+  </si>
+  <si>
+    <t>01:47:25:145</t>
+  </si>
+  <si>
+    <t>TR20240731014725250</t>
+  </si>
+  <si>
+    <t>01:47:25:251</t>
+  </si>
+  <si>
+    <t>TR20240731014725359</t>
+  </si>
+  <si>
+    <t>01:47:25:360</t>
+  </si>
+  <si>
+    <t>TR20240730015409284</t>
+  </si>
+  <si>
+    <t>01:54:09:284</t>
+  </si>
+  <si>
+    <t>TR20240730015409392</t>
+  </si>
+  <si>
+    <t>01:54:09:392</t>
+  </si>
+  <si>
+    <t>TR20240730015409501</t>
+  </si>
+  <si>
+    <t>01:54:09:501</t>
+  </si>
+  <si>
+    <t>TR20240731015409611</t>
+  </si>
+  <si>
+    <t>01:54:09:612</t>
+  </si>
+  <si>
+    <t>TR20240731015409720</t>
+  </si>
+  <si>
+    <t>01:54:09:720</t>
   </si>
 </sst>
 </file>
@@ -2810,16 +3053,16 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>780</v>
+        <v>861</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>629</v>
+        <v>636</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>781</v>
+        <v>862</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>15</v>
@@ -2860,16 +3103,16 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>782</v>
+        <v>863</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>629</v>
+        <v>636</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>783</v>
+        <v>864</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>16</v>
@@ -2910,16 +3153,16 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>784</v>
+        <v>865</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>629</v>
+        <v>636</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>785</v>
+        <v>866</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>17</v>
@@ -2960,16 +3203,16 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>786</v>
+        <v>867</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>636</v>
+        <v>797</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>787</v>
+        <v>868</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>42</v>
@@ -3010,16 +3253,16 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>788</v>
+        <v>869</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>636</v>
+        <v>797</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>789</v>
+        <v>870</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>41</v>

</xml_diff>